<commit_message>
Added testdata, xls, argument files, validation files and robot files for all three apis.
</commit_message>
<xml_diff>
--- a/XlsFiles/CustomerConfigs.xlsx
+++ b/XlsFiles/CustomerConfigs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Cutomer Id</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>Addresses</t>
+  </si>
+  <si>
+    <t>CUST1</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>DT11</t>
+  </si>
+  <si>
+    <t>addr1</t>
   </si>
 </sst>
 </file>
@@ -349,10 +361,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,33 +417,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>